<commit_message>
Irfan - Updated graphs for the report. Mostly just adding labels and adjusting axis. No data changes.
</commit_message>
<xml_diff>
--- a/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
+++ b/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Source\Repos\ECE1718H\goldendata\Assigment3_E1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikhan1\Source\Repo_1\ECE1718H\goldendata\Assigment3_E1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CIF - bitcount" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -139,15 +139,26 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Bitcount per</a:t>
+              <a:t>CIF Bitcount per Frame</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rate</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frame - CIF Rate Control</a:t>
+              <a:t> Control with 2.4 mbps Target Bitrate</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -294,7 +305,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8073-48B5-8EBC-7D949E03E640}"/>
             </c:ext>
@@ -411,7 +422,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8073-48B5-8EBC-7D949E03E640}"/>
             </c:ext>
@@ -528,7 +539,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8073-48B5-8EBC-7D949E03E640}"/>
             </c:ext>
@@ -544,16 +555,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="371754352"/>
+        <c:axId val="371746904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="371754352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -590,7 +657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="371746904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,9 +665,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="371746904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="60000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -618,6 +686,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bitcount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -649,7 +773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="371754352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -662,7 +786,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -730,7 +855,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -764,16 +889,33 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Bitcount per</a:t>
+              <a:t>QCIF</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frame - QCIF Rate Control</a:t>
+              <a:t> Bitcount Per Frame</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rate Control with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 960 kbps Target Bitrate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -920,7 +1062,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2401-4774-B09A-99796626A598}"/>
             </c:ext>
@@ -1037,7 +1179,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2401-4774-B09A-99796626A598}"/>
             </c:ext>
@@ -1154,7 +1296,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2401-4774-B09A-99796626A598}"/>
             </c:ext>
@@ -1170,16 +1312,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="371748080"/>
+        <c:axId val="371753176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="371748080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1216,7 +1414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="371753176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1224,9 +1422,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="371753176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="20000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1244,6 +1443,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bitcount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1275,7 +1530,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="371748080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1288,7 +1543,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1356,7 +1612,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1390,16 +1646,28 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>PSRN per</a:t>
+              <a:t>CIF PSNR per Frame</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frame - CIF Rate Control</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Rate Control with 2.4 mbps Target Bitrate</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2456559596717077"/>
+          <c:y val="3.9753528125621149E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1546,7 +1814,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6A2C-4216-BE11-04657B9942C4}"/>
             </c:ext>
@@ -1663,7 +1931,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6A2C-4216-BE11-04657B9942C4}"/>
             </c:ext>
@@ -1780,7 +2048,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6A2C-4216-BE11-04657B9942C4}"/>
             </c:ext>
@@ -1796,16 +2064,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="373191904"/>
+        <c:axId val="373194256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="373191904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1842,7 +2166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="373194256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1850,9 +2174,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="373194256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="15"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1870,6 +2195,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PSNR (dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1901,7 +2282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="373191904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1914,7 +2295,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25405457651126945"/>
+          <c:y val="0.88175623496818645"/>
+          <c:w val="0.52575328083989503"/>
+          <c:h val="6.9103700046979716E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1982,7 +2373,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2016,16 +2407,21 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>PSRN per</a:t>
+              <a:t>QCIF PSNR per Frame</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frame - QCIF Rate Control</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Rate Control with 960 kbps Target Bitrate</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2172,7 +2568,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-198D-4628-9217-65C85412046C}"/>
             </c:ext>
@@ -2289,7 +2685,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-198D-4628-9217-65C85412046C}"/>
             </c:ext>
@@ -2406,7 +2802,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-198D-4628-9217-65C85412046C}"/>
             </c:ext>
@@ -2422,16 +2818,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="373194648"/>
+        <c:axId val="373192296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="373194648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2468,7 +2920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="373192296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2476,9 +2928,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="373192296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="15"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2496,6 +2949,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PSNR</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (dB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2527,7 +3041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="373194648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2540,7 +3054,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2608,7 +3123,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2642,15 +3157,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Bitcount per</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frame I-Period_21</a:t>
+              <a:t>CIF Bitcount per Frame with I_Period 21</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2789,7 +3301,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C7DA-46B0-B3A4-E291B99D355C}"/>
             </c:ext>
@@ -2898,7 +3410,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C7DA-46B0-B3A4-E291B99D355C}"/>
             </c:ext>
@@ -2914,16 +3426,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="373196216"/>
+        <c:axId val="373193864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="373196216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2960,7 +3528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="373193864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2968,7 +3536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="373193864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2988,6 +3556,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bitcount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3019,7 +3643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="373196216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3032,7 +3656,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3100,7 +3725,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3133,17 +3758,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>PSNR per Frame I-Period_21</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>CIF PSNR per Frame I-Period_21</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3282,7 +3903,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F713-4D6A-9FA3-E860749E504A}"/>
             </c:ext>
@@ -3391,7 +4012,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F713-4D6A-9FA3-E860749E504A}"/>
             </c:ext>
@@ -3407,16 +4028,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="472469928"/>
-        <c:axId val="472471568"/>
+        <c:axId val="373197392"/>
+        <c:axId val="373196608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472469928"/>
+        <c:axId val="373197392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3453,7 +4130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472471568"/>
+        <c:crossAx val="373196608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3461,9 +4138,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472471568"/>
+        <c:axId val="373196608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3481,6 +4159,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PSNR (dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3512,7 +4246,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472469928"/>
+        <c:crossAx val="373197392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3525,7 +4259,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6854,23 +7589,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>33336</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>172402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>528637</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{142B6B42-A60F-40C3-B7D9-6E595AF55735}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{142B6B42-A60F-40C3-B7D9-6E595AF55735}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6896,22 +7631,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>581024</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6280FB-87F9-405C-A090-61ADA31C9807}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F6280FB-87F9-405C-A090-61ADA31C9807}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6940,21 +7675,21 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>83819</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D04CAEE3-0F90-4EA5-AE66-F3F142605586}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D04CAEE3-0F90-4EA5-AE66-F3F142605586}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6982,22 +7717,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2FA466A-6EE6-4C88-8D4D-43D014D8EF0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A2FA466A-6EE6-4C88-8D4D-43D014D8EF0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7024,23 +7759,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>121919</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE3E938-8689-4F50-883F-C57EE6C3B466}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACE3E938-8689-4F50-883F-C57EE6C3B466}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7073,17 +7808,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DADDA05-2F4D-4CC4-8AA5-CEAA532A74AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DADDA05-2F4D-4CC4-8AA5-CEAA532A74AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7405,13 +8140,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7422,7 +8157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7442,7 +8177,7 @@
         <v>81342</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7462,7 +8197,7 @@
         <v>78199</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7482,7 +8217,7 @@
         <v>81695</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7502,7 +8237,7 @@
         <v>81021</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7522,7 +8257,7 @@
         <v>79009</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7542,7 +8277,7 @@
         <v>81037</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7562,7 +8297,7 @@
         <v>79972</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7582,7 +8317,7 @@
         <v>80522</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7602,7 +8337,7 @@
         <v>79832</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7622,7 +8357,7 @@
         <v>81977</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7642,7 +8377,7 @@
         <v>76938</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7662,7 +8397,7 @@
         <v>81716</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7682,7 +8417,7 @@
         <v>73925</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7702,7 +8437,7 @@
         <v>82606</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -7722,7 +8457,7 @@
         <v>81339</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -7742,7 +8477,7 @@
         <v>80225</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -7762,7 +8497,7 @@
         <v>80798</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -7782,7 +8517,7 @@
         <v>84661</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -7802,7 +8537,7 @@
         <v>82641</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -7822,7 +8557,7 @@
         <v>81634</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -7853,12 +8588,12 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7869,7 +8604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7889,7 +8624,7 @@
         <v>31324</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7909,7 +8644,7 @@
         <v>31651</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7929,7 +8664,7 @@
         <v>32240</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7949,7 +8684,7 @@
         <v>31098</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7969,7 +8704,7 @@
         <v>31407</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7989,7 +8724,7 @@
         <v>31751</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8009,7 +8744,7 @@
         <v>32790</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8029,7 +8764,7 @@
         <v>32421</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8049,7 +8784,7 @@
         <v>33397</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8069,7 +8804,7 @@
         <v>31886</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8089,7 +8824,7 @@
         <v>34355</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8109,7 +8844,7 @@
         <v>32826</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8129,7 +8864,7 @@
         <v>30940</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8149,7 +8884,7 @@
         <v>26603</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8169,7 +8904,7 @@
         <v>52535</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -8189,7 +8924,7 @@
         <v>32219</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -8209,7 +8944,7 @@
         <v>31424</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -8229,7 +8964,7 @@
         <v>31743</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -8249,7 +8984,7 @@
         <v>33054</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -8269,7 +9004,7 @@
         <v>32373</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8300,12 +9035,12 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8316,7 +9051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8336,7 +9071,7 @@
         <v>32.922676000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8356,7 +9091,7 @@
         <v>32.792614</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8376,7 +9111,7 @@
         <v>33.232483000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8396,7 +9131,7 @@
         <v>33.418678</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8416,7 +9151,7 @@
         <v>33.284270999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8436,7 +9171,7 @@
         <v>33.123874999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8456,7 +9191,7 @@
         <v>33.753342000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8476,7 +9211,7 @@
         <v>22.994844000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8496,7 +9231,7 @@
         <v>29.168758</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8516,7 +9251,7 @@
         <v>32.136276000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8536,7 +9271,7 @@
         <v>33.205719000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8556,7 +9291,7 @@
         <v>34.017895000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8576,7 +9311,7 @@
         <v>34.439681999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8596,7 +9331,7 @@
         <v>34.759304</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8616,7 +9351,7 @@
         <v>20.805440999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -8636,7 +9371,7 @@
         <v>25.39809</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -8656,7 +9391,7 @@
         <v>27.031410000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -8676,7 +9411,7 @@
         <v>28.770468000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -8696,7 +9431,7 @@
         <v>29.359988999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -8716,7 +9451,7 @@
         <v>29.705095</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8750,9 +9485,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8763,7 +9498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8783,7 +9518,7 @@
         <v>32.892646999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8803,7 +9538,7 @@
         <v>33.456001000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8823,7 +9558,7 @@
         <v>34.168976000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8843,7 +9578,7 @@
         <v>34.502116999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8863,7 +9598,7 @@
         <v>34.494083000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8883,7 +9618,7 @@
         <v>34.523617000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8903,7 +9638,7 @@
         <v>35.091895999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8923,7 +9658,7 @@
         <v>24.018940000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8943,7 +9678,7 @@
         <v>30.361965000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8963,7 +9698,7 @@
         <v>32.183281000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8983,7 +9718,7 @@
         <v>34.727454999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -9003,7 +9738,7 @@
         <v>35.920475000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9023,7 +9758,7 @@
         <v>36.406334000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9043,7 +9778,7 @@
         <v>36.957703000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9063,7 +9798,7 @@
         <v>21.222179000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -9083,7 +9818,7 @@
         <v>26.213009</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -9103,7 +9838,7 @@
         <v>28.358971</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -9123,7 +9858,7 @@
         <v>29.705147</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -9143,7 +9878,7 @@
         <v>30.502040999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -9163,7 +9898,7 @@
         <v>30.806025999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -9193,13 +9928,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -9210,7 +9945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
@@ -9251,7 +9986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -9283,7 +10018,7 @@
         <v>81342</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9315,7 +10050,7 @@
         <v>78199</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -9347,7 +10082,7 @@
         <v>81695</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -9379,7 +10114,7 @@
         <v>81021</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -9411,7 +10146,7 @@
         <v>79009</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -9443,7 +10178,7 @@
         <v>81037</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -9475,7 +10210,7 @@
         <v>79972</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -9507,7 +10242,7 @@
         <v>80522</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -9539,7 +10274,7 @@
         <v>79832</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -9571,7 +10306,7 @@
         <v>81977</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -9603,7 +10338,7 @@
         <v>76938</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -9635,7 +10370,7 @@
         <v>81716</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9667,7 +10402,7 @@
         <v>73925</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -9699,7 +10434,7 @@
         <v>82606</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -9731,7 +10466,7 @@
         <v>81339</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -9763,7 +10498,7 @@
         <v>80225</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -9795,7 +10530,7 @@
         <v>80798</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -9827,7 +10562,7 @@
         <v>84661</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -9859,7 +10594,7 @@
         <v>82641</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -9891,7 +10626,7 @@
         <v>81634</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -9923,7 +10658,7 @@
         <v>80497</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24">
         <f>SUM(B3:B23)</f>
         <v>7528643</v>
@@ -9985,7 +10720,7 @@
         <v>1691586</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25">
         <f>P24/B24</f>
         <v>0.22468670648880548</v>
@@ -10025,13 +10760,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -10042,7 +10777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10053,7 +10788,7 @@
         <v>32.922676000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10064,7 +10799,7 @@
         <v>32.792614</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -10075,7 +10810,7 @@
         <v>33.232483000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -10086,7 +10821,7 @@
         <v>33.418678</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -10097,7 +10832,7 @@
         <v>33.284270999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -10108,7 +10843,7 @@
         <v>33.123874999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -10119,7 +10854,7 @@
         <v>33.753342000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -10130,7 +10865,7 @@
         <v>22.994844000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -10141,7 +10876,7 @@
         <v>29.168758</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -10152,7 +10887,7 @@
         <v>32.136276000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -10163,7 +10898,7 @@
         <v>33.205719000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -10174,7 +10909,7 @@
         <v>34.017895000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -10185,7 +10920,7 @@
         <v>34.439681999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -10196,7 +10931,7 @@
         <v>34.759304</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -10207,7 +10942,7 @@
         <v>20.805440999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -10218,7 +10953,7 @@
         <v>25.39809</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -10229,7 +10964,7 @@
         <v>27.031410000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -10240,7 +10975,7 @@
         <v>28.770468000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -10251,7 +10986,7 @@
         <v>29.359988999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -10262,7 +10997,7 @@
         <v>29.705095</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
fixing bug with rate control and update graphs
</commit_message>
<xml_diff>
--- a/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
+++ b/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Source\Repos\ECE1718H\goldendata\Assigment3_E1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CIF - bitcount" sheetId="1" r:id="rId1"/>
@@ -231,64 +231,64 @@
                   <c:v>81342</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83421</c:v>
+                  <c:v>84595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83438</c:v>
+                  <c:v>80962</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83654</c:v>
+                  <c:v>82299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83823</c:v>
+                  <c:v>80978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83061</c:v>
+                  <c:v>83020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80278</c:v>
+                  <c:v>80925</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77594</c:v>
+                  <c:v>77491</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77068</c:v>
+                  <c:v>75549</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78766</c:v>
+                  <c:v>75578</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>78626</c:v>
+                  <c:v>77700</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>78581</c:v>
+                  <c:v>76962</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78908</c:v>
+                  <c:v>76412</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>78545</c:v>
+                  <c:v>76591</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>82980</c:v>
+                  <c:v>83125</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>80967</c:v>
+                  <c:v>82578</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83880</c:v>
+                  <c:v>82174</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79939</c:v>
+                  <c:v>83413</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>80709</c:v>
+                  <c:v>83933</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81513</c:v>
+                  <c:v>83668</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>82126</c:v>
+                  <c:v>80411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,64 +348,64 @@
                   <c:v>81342</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78199</c:v>
+                  <c:v>79228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81695</c:v>
+                  <c:v>83375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81021</c:v>
+                  <c:v>79187</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83823</c:v>
+                  <c:v>80978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78171</c:v>
+                  <c:v>78584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80134</c:v>
+                  <c:v>77552</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80059</c:v>
+                  <c:v>80013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77068</c:v>
+                  <c:v>75549</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>74409</c:v>
+                  <c:v>74458</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>73624</c:v>
+                  <c:v>68403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>72091</c:v>
+                  <c:v>64749</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78908</c:v>
+                  <c:v>76412</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>76290</c:v>
+                  <c:v>73323</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>122776</c:v>
+                  <c:v>80796</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>79490</c:v>
+                  <c:v>81326</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83880</c:v>
+                  <c:v>82174</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80757</c:v>
+                  <c:v>81990</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>84001</c:v>
+                  <c:v>82465</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>83352</c:v>
+                  <c:v>81220</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>82126</c:v>
+                  <c:v>80411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -465,64 +465,64 @@
                   <c:v>81342</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78199</c:v>
+                  <c:v>79228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81695</c:v>
+                  <c:v>83375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81021</c:v>
+                  <c:v>79187</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79009</c:v>
+                  <c:v>83509</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81037</c:v>
+                  <c:v>82348</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>79972</c:v>
+                  <c:v>78191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80522</c:v>
+                  <c:v>80028</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79832</c:v>
+                  <c:v>80060</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81977</c:v>
+                  <c:v>81075</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76938</c:v>
+                  <c:v>83297</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>81716</c:v>
+                  <c:v>71991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73925</c:v>
+                  <c:v>77777</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>82606</c:v>
+                  <c:v>73438</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81339</c:v>
+                  <c:v>80727</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>80225</c:v>
+                  <c:v>83899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80798</c:v>
+                  <c:v>84656</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>84661</c:v>
+                  <c:v>80427</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82641</c:v>
+                  <c:v>82393</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81634</c:v>
+                  <c:v>81979</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80497</c:v>
+                  <c:v>85330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -857,64 +857,64 @@
                   <c:v>31324</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31502</c:v>
+                  <c:v>30939</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31696</c:v>
+                  <c:v>31214</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31765</c:v>
+                  <c:v>31400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32071</c:v>
+                  <c:v>31764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31714</c:v>
+                  <c:v>32130</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32238</c:v>
+                  <c:v>31145</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30294</c:v>
+                  <c:v>31572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30265</c:v>
+                  <c:v>32031</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30907</c:v>
+                  <c:v>31875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30705</c:v>
+                  <c:v>31905</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30553</c:v>
+                  <c:v>31700</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30610</c:v>
+                  <c:v>31855</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30679</c:v>
+                  <c:v>30134</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32126</c:v>
+                  <c:v>31725</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31387</c:v>
+                  <c:v>31970</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32671</c:v>
+                  <c:v>32078</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32542</c:v>
+                  <c:v>32381</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32337</c:v>
+                  <c:v>31587</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32326</c:v>
+                  <c:v>31602</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32467</c:v>
+                  <c:v>32207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,64 +974,64 @@
                   <c:v>31324</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31651</c:v>
+                  <c:v>31977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32240</c:v>
+                  <c:v>31787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31098</c:v>
+                  <c:v>32347</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32071</c:v>
+                  <c:v>31764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30555</c:v>
+                  <c:v>30874</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30749</c:v>
+                  <c:v>30067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31997</c:v>
+                  <c:v>32037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30265</c:v>
+                  <c:v>32031</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32920</c:v>
+                  <c:v>27933</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28797</c:v>
+                  <c:v>29900</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26747</c:v>
+                  <c:v>24117</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30610</c:v>
+                  <c:v>31855</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30576</c:v>
+                  <c:v>28018</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32500</c:v>
+                  <c:v>32249</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31960</c:v>
+                  <c:v>33410</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>32078</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>32671</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>32546</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>31626</c:v>
+                  <c:v>32300</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32290</c:v>
+                  <c:v>31386</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32467</c:v>
+                  <c:v>32207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,64 +1091,64 @@
                   <c:v>31324</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31651</c:v>
+                  <c:v>31977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32240</c:v>
+                  <c:v>31787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31098</c:v>
+                  <c:v>32347</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31407</c:v>
+                  <c:v>31369</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31751</c:v>
+                  <c:v>32987</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32790</c:v>
+                  <c:v>30597</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32421</c:v>
+                  <c:v>32213</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33397</c:v>
+                  <c:v>32296</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31886</c:v>
+                  <c:v>33528</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34355</c:v>
+                  <c:v>35328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32826</c:v>
+                  <c:v>32199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30940</c:v>
+                  <c:v>26898</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26603</c:v>
+                  <c:v>23635</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52535</c:v>
+                  <c:v>32362</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32219</c:v>
+                  <c:v>32362</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31424</c:v>
+                  <c:v>34667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31743</c:v>
+                  <c:v>30961</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33054</c:v>
+                  <c:v>31734</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32373</c:v>
+                  <c:v>34462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32286</c:v>
+                  <c:v>32727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1483,64 +1483,64 @@
                   <c:v>32.922676000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.373069999999998</c:v>
+                  <c:v>33.065178000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.095580999999999</c:v>
+                  <c:v>33.111407999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.294239000000001</c:v>
+                  <c:v>33.247089000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.085417</c:v>
+                  <c:v>33.061886000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.188818000000001</c:v>
+                  <c:v>33.189579000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.16696</c:v>
+                  <c:v>32.990250000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.570141</c:v>
+                  <c:v>37.519649999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.549689999999998</c:v>
+                  <c:v>37.477913000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.718273000000003</c:v>
+                  <c:v>37.431870000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.736449999999998</c:v>
+                  <c:v>37.536411000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.768166000000001</c:v>
+                  <c:v>37.600158999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.814216999999999</c:v>
+                  <c:v>37.764488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.797150000000002</c:v>
+                  <c:v>37.750587000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30.933146000000001</c:v>
+                  <c:v>32.999721999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31.153697999999999</c:v>
+                  <c:v>32.989418000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.899647000000002</c:v>
+                  <c:v>32.905132000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.831762000000001</c:v>
+                  <c:v>32.944232999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.786688000000002</c:v>
+                  <c:v>32.892417999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.791183</c:v>
+                  <c:v>32.676471999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.580539999999999</c:v>
+                  <c:v>32.626807999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,64 +1600,64 @@
                   <c:v>32.922676000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.792614</c:v>
+                  <c:v>33.977221999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.232483000000002</c:v>
+                  <c:v>34.17915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.418678</c:v>
+                  <c:v>34.373299000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.085417</c:v>
+                  <c:v>33.061886000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.239235000000001</c:v>
+                  <c:v>34.032668999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.238807999999999</c:v>
+                  <c:v>34.421059</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.919419999999999</c:v>
+                  <c:v>23.96011</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.549689999999998</c:v>
+                  <c:v>37.477913000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.256050000000002</c:v>
+                  <c:v>39.012096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.004283999999998</c:v>
+                  <c:v>39.414776000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39.247245999999997</c:v>
+                  <c:v>39.556972999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.814216999999999</c:v>
+                  <c:v>37.764488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.412365000000001</c:v>
+                  <c:v>39.167709000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.073996999999999</c:v>
+                  <c:v>22.779028</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.352744999999999</c:v>
+                  <c:v>27.471257999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.899647000000002</c:v>
+                  <c:v>32.905132000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.086844999999997</c:v>
+                  <c:v>33.956333000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.393700000000003</c:v>
+                  <c:v>34.035122000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.549030000000002</c:v>
+                  <c:v>34.061698999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.580539999999999</c:v>
+                  <c:v>32.626807999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,64 +1717,64 @@
                   <c:v>32.922676000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.792614</c:v>
+                  <c:v>33.977221999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.232483000000002</c:v>
+                  <c:v>34.17915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.418678</c:v>
+                  <c:v>34.373299000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.284270999999997</c:v>
+                  <c:v>34.428963000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.123874999999998</c:v>
+                  <c:v>34.163581999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.753342000000004</c:v>
+                  <c:v>34.500087999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.994844000000001</c:v>
+                  <c:v>23.703171000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.168758</c:v>
+                  <c:v>28.713322000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.136276000000002</c:v>
+                  <c:v>30.99127</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.205719000000002</c:v>
+                  <c:v>32.092789000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.017895000000003</c:v>
+                  <c:v>32.687973</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.439681999999998</c:v>
+                  <c:v>33.095160999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.759304</c:v>
+                  <c:v>33.323334000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.805440999999998</c:v>
+                  <c:v>22.738938999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25.39809</c:v>
+                  <c:v>27.305260000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.031410000000001</c:v>
+                  <c:v>28.801749999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28.770468000000001</c:v>
+                  <c:v>29.536162999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.359988999999999</c:v>
+                  <c:v>30.126584999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.705095</c:v>
+                  <c:v>30.388870000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.865494000000002</c:v>
+                  <c:v>30.692335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,64 +2109,64 @@
                   <c:v>32.892646999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.850273000000001</c:v>
+                  <c:v>32.881531000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.829595999999999</c:v>
+                  <c:v>32.986404</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.877098</c:v>
+                  <c:v>32.931587</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.718741999999999</c:v>
+                  <c:v>32.914935999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.699404000000001</c:v>
+                  <c:v>32.921638000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.683685000000001</c:v>
+                  <c:v>32.868858000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.040691000000002</c:v>
+                  <c:v>36.172652999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.052055000000003</c:v>
+                  <c:v>36.181156000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.014301000000003</c:v>
+                  <c:v>36.166392999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.010815000000001</c:v>
+                  <c:v>36.141379999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.026440000000001</c:v>
+                  <c:v>36.221694999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.042693999999997</c:v>
+                  <c:v>36.197647000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.995995000000001</c:v>
+                  <c:v>35.967609000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.619909</c:v>
+                  <c:v>32.800026000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.190318999999999</c:v>
+                  <c:v>32.793658999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.182279999999999</c:v>
+                  <c:v>32.833832000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.235727000000001</c:v>
+                  <c:v>32.843178000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.139481</c:v>
+                  <c:v>32.300201000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.256661999999999</c:v>
+                  <c:v>32.285674999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.063071999999998</c:v>
+                  <c:v>32.268013000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,64 +2226,64 @@
                   <c:v>32.892646999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.456001000000001</c:v>
+                  <c:v>34.352325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.168976000000001</c:v>
+                  <c:v>35.006332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.502116999999998</c:v>
+                  <c:v>35.557068000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.718741999999999</c:v>
+                  <c:v>32.914935999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.801926000000002</c:v>
+                  <c:v>34.665264000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.135883</c:v>
+                  <c:v>35.458809000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.665482000000001</c:v>
+                  <c:v>23.881233000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.052055000000003</c:v>
+                  <c:v>36.181156000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.925635999999997</c:v>
+                  <c:v>38.439255000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.509425999999998</c:v>
+                  <c:v>39.893386999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.210692999999999</c:v>
+                  <c:v>40.327922999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.042693999999997</c:v>
+                  <c:v>36.197647000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.853518999999999</c:v>
+                  <c:v>38.604725000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.299306999999999</c:v>
+                  <c:v>23.920334</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.367775000000002</c:v>
+                  <c:v>28.541819</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.182279999999999</c:v>
+                  <c:v>32.833832000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.058422</c:v>
+                  <c:v>34.511825999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.7729</c:v>
+                  <c:v>34.956394000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.134014000000001</c:v>
+                  <c:v>34.556598999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.063071999999998</c:v>
+                  <c:v>32.268013000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2343,64 +2343,64 @@
                   <c:v>32.892646999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.456001000000001</c:v>
+                  <c:v>34.352325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.168976000000001</c:v>
+                  <c:v>35.006332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.502116999999998</c:v>
+                  <c:v>35.557068000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.494083000000003</c:v>
+                  <c:v>35.637794</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.523617000000002</c:v>
+                  <c:v>35.687389000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.091895999999998</c:v>
+                  <c:v>35.914794999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.018940000000001</c:v>
+                  <c:v>24.539190000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.361965000000001</c:v>
+                  <c:v>28.903199999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.183281000000001</c:v>
+                  <c:v>33.032898000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.727454999999999</c:v>
+                  <c:v>34.301861000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.920475000000003</c:v>
+                  <c:v>34.770195000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.406334000000001</c:v>
+                  <c:v>35.139763000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.957703000000002</c:v>
+                  <c:v>35.203026000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.222179000000001</c:v>
+                  <c:v>23.242861000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.213009</c:v>
+                  <c:v>27.613441000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.358971</c:v>
+                  <c:v>29.790945000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.705147</c:v>
+                  <c:v>30.262892000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.502040999999998</c:v>
+                  <c:v>30.463058</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.806025999999999</c:v>
+                  <c:v>31.125328</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.855761000000001</c:v>
+                  <c:v>31.308893000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2726,64 +2726,64 @@
                   <c:v>81342</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78199</c:v>
+                  <c:v>79228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81695</c:v>
+                  <c:v>83375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81021</c:v>
+                  <c:v>79187</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79009</c:v>
+                  <c:v>83509</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81037</c:v>
+                  <c:v>82348</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>79972</c:v>
+                  <c:v>78191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80522</c:v>
+                  <c:v>80028</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79832</c:v>
+                  <c:v>80060</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81977</c:v>
+                  <c:v>81075</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76938</c:v>
+                  <c:v>83297</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>81716</c:v>
+                  <c:v>71991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73925</c:v>
+                  <c:v>77777</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>82606</c:v>
+                  <c:v>73438</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81339</c:v>
+                  <c:v>80727</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>80225</c:v>
+                  <c:v>83899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80798</c:v>
+                  <c:v>84656</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>84661</c:v>
+                  <c:v>80427</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82641</c:v>
+                  <c:v>82393</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81634</c:v>
+                  <c:v>81979</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80497</c:v>
+                  <c:v>85330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3219,64 +3219,64 @@
                   <c:v>32.922676000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.792614</c:v>
+                  <c:v>33.977221999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.232483000000002</c:v>
+                  <c:v>34.17915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.418678</c:v>
+                  <c:v>34.373299000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.284270999999997</c:v>
+                  <c:v>34.428963000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.123874999999998</c:v>
+                  <c:v>34.163581999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.753342000000004</c:v>
+                  <c:v>34.500087999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.994844000000001</c:v>
+                  <c:v>23.703171000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.168758</c:v>
+                  <c:v>28.713322000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.136276000000002</c:v>
+                  <c:v>30.99127</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.205719000000002</c:v>
+                  <c:v>32.092789000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.017895000000003</c:v>
+                  <c:v>32.687973</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.439681999999998</c:v>
+                  <c:v>33.095160999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.759304</c:v>
+                  <c:v>33.323334000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.805440999999998</c:v>
+                  <c:v>22.738938999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25.39809</c:v>
+                  <c:v>27.305260000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.031410000000001</c:v>
+                  <c:v>28.801749999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28.770468000000001</c:v>
+                  <c:v>29.536162999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.359988999999999</c:v>
+                  <c:v>30.126584999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.705095</c:v>
+                  <c:v>30.388870000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.865494000000002</c:v>
+                  <c:v>30.692335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7024,16 +7024,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7447,19 +7447,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>83421</v>
+        <v>84595</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>78199</v>
+        <v>79228</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>78199</v>
+        <v>79228</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7467,19 +7467,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>83438</v>
+        <v>80962</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>81695</v>
+        <v>83375</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>81695</v>
+        <v>83375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7487,19 +7487,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>83654</v>
+        <v>82299</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>81021</v>
+        <v>79187</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>81021</v>
+        <v>79187</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7507,19 +7507,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>83823</v>
+        <v>80978</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>83823</v>
+        <v>80978</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>79009</v>
+        <v>83509</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7527,19 +7527,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>83061</v>
+        <v>83020</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>78171</v>
+        <v>78584</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>81037</v>
+        <v>82348</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7547,19 +7547,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>80278</v>
+        <v>80925</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>80134</v>
+        <v>77552</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>79972</v>
+        <v>78191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7567,19 +7567,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>77594</v>
+        <v>77491</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>80059</v>
+        <v>80013</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>80522</v>
+        <v>80028</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7587,19 +7587,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>77068</v>
+        <v>75549</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>77068</v>
+        <v>75549</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>79832</v>
+        <v>80060</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -7607,19 +7607,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>78766</v>
+        <v>75578</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>74409</v>
+        <v>74458</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>81977</v>
+        <v>81075</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -7627,19 +7627,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>78626</v>
+        <v>77700</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>73624</v>
+        <v>68403</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>76938</v>
+        <v>83297</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -7647,19 +7647,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>78581</v>
+        <v>76962</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>72091</v>
+        <v>64749</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>81716</v>
+        <v>71991</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -7667,19 +7667,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78908</v>
+        <v>76412</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>78908</v>
+        <v>76412</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>73925</v>
+        <v>77777</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -7687,19 +7687,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78545</v>
+        <v>76591</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>76290</v>
+        <v>73323</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>82606</v>
+        <v>73438</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7707,19 +7707,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82980</v>
+        <v>83125</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>122776</v>
+        <v>80796</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>81339</v>
+        <v>80727</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -7727,19 +7727,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>80967</v>
+        <v>82578</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>79490</v>
+        <v>81326</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>80225</v>
+        <v>83899</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -7747,19 +7747,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83880</v>
+        <v>82174</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>83880</v>
+        <v>82174</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>80798</v>
+        <v>84656</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -7767,19 +7767,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>79939</v>
+        <v>83413</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>80757</v>
+        <v>81990</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>84661</v>
+        <v>80427</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -7787,19 +7787,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>80709</v>
+        <v>83933</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>84001</v>
+        <v>82465</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>82641</v>
+        <v>82393</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -7807,19 +7807,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>81513</v>
+        <v>83668</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>83352</v>
+        <v>81220</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>81634</v>
+        <v>81979</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -7827,19 +7827,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>82126</v>
+        <v>80411</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>82126</v>
+        <v>80411</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>80497</v>
+        <v>85330</v>
       </c>
     </row>
   </sheetData>
@@ -7853,7 +7853,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7894,19 +7894,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>31502</v>
+        <v>30939</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>31651</v>
+        <v>31977</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>31651</v>
+        <v>31977</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7914,19 +7914,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>31696</v>
+        <v>31214</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>32240</v>
+        <v>31787</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>32240</v>
+        <v>31787</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7934,19 +7934,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>31765</v>
+        <v>31400</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>31098</v>
+        <v>32347</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>31098</v>
+        <v>32347</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7954,19 +7954,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>32071</v>
+        <v>31764</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>32071</v>
+        <v>31764</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>31407</v>
+        <v>31369</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7974,19 +7974,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>31714</v>
+        <v>32130</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>30555</v>
+        <v>30874</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>31751</v>
+        <v>32987</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7994,19 +7994,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>32238</v>
+        <v>31145</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>30749</v>
+        <v>30067</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>32790</v>
+        <v>30597</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8014,19 +8014,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>30294</v>
+        <v>31572</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>31997</v>
+        <v>32037</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>32421</v>
+        <v>32213</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8034,19 +8034,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>30265</v>
+        <v>32031</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>30265</v>
+        <v>32031</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>33397</v>
+        <v>32296</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8054,19 +8054,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>30907</v>
+        <v>31875</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>32920</v>
+        <v>27933</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>31886</v>
+        <v>33528</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8074,19 +8074,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>30705</v>
+        <v>31905</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>28797</v>
+        <v>29900</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>34355</v>
+        <v>35328</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8094,19 +8094,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>30553</v>
+        <v>31700</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>26747</v>
+        <v>24117</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>32826</v>
+        <v>32199</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8114,19 +8114,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>30610</v>
+        <v>31855</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>30610</v>
+        <v>31855</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>30940</v>
+        <v>26898</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8134,19 +8134,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>30679</v>
+        <v>30134</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>30576</v>
+        <v>28018</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>26603</v>
+        <v>23635</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8154,19 +8154,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>32126</v>
+        <v>31725</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>32500</v>
+        <v>32249</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>52535</v>
+        <v>32362</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8174,19 +8174,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>31387</v>
+        <v>31970</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>31960</v>
+        <v>33410</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>32219</v>
+        <v>32362</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8194,19 +8194,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>32671</v>
+        <v>32078</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>32671</v>
+        <v>32078</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>31424</v>
+        <v>34667</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8214,19 +8214,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>32542</v>
+        <v>32381</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>32546</v>
+        <v>32671</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>31743</v>
+        <v>30961</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -8234,19 +8234,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>32337</v>
+        <v>31587</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>31626</v>
+        <v>32300</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>33054</v>
+        <v>31734</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -8254,19 +8254,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>32326</v>
+        <v>31602</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>32290</v>
+        <v>31386</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>32373</v>
+        <v>34462</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -8274,19 +8274,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>32467</v>
+        <v>32207</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>32467</v>
+        <v>32207</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>32286</v>
+        <v>32727</v>
       </c>
     </row>
   </sheetData>
@@ -8341,19 +8341,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>31.373069999999998</v>
+        <v>33.065178000000003</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>32.792614</v>
+        <v>33.977221999999998</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>32.792614</v>
+        <v>33.977221999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8361,19 +8361,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>31.095580999999999</v>
+        <v>33.111407999999997</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>33.232483000000002</v>
+        <v>34.17915</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>33.232483000000002</v>
+        <v>34.17915</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8381,19 +8381,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>31.294239000000001</v>
+        <v>33.247089000000003</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>33.418678</v>
+        <v>34.373299000000003</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>33.418678</v>
+        <v>34.373299000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8401,19 +8401,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>31.085417</v>
+        <v>33.061886000000001</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>31.085417</v>
+        <v>33.061886000000001</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>33.284270999999997</v>
+        <v>34.428963000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8421,19 +8421,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>31.188818000000001</v>
+        <v>33.189579000000002</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>32.239235000000001</v>
+        <v>34.032668999999999</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>33.123874999999998</v>
+        <v>34.163581999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8441,19 +8441,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>31.16696</v>
+        <v>32.990250000000003</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>33.238807999999999</v>
+        <v>34.421059</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>33.753342000000004</v>
+        <v>34.500087999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8461,19 +8461,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>36.570141</v>
+        <v>37.519649999999999</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>22.919419999999999</v>
+        <v>23.96011</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>22.994844000000001</v>
+        <v>23.703171000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8481,19 +8481,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>36.549689999999998</v>
+        <v>37.477913000000001</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>36.549689999999998</v>
+        <v>37.477913000000001</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>29.168758</v>
+        <v>28.713322000000002</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8501,19 +8501,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>36.718273000000003</v>
+        <v>37.431870000000004</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>38.256050000000002</v>
+        <v>39.012096</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>32.136276000000002</v>
+        <v>30.99127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8521,19 +8521,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>36.736449999999998</v>
+        <v>37.536411000000001</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>39.004283999999998</v>
+        <v>39.414776000000003</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>33.205719000000002</v>
+        <v>32.092789000000003</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8541,19 +8541,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>36.768166000000001</v>
+        <v>37.600158999999998</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>39.247245999999997</v>
+        <v>39.556972999999999</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>34.017895000000003</v>
+        <v>32.687973</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8561,19 +8561,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>36.814216999999999</v>
+        <v>37.764488</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>36.814216999999999</v>
+        <v>37.764488</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>34.439681999999998</v>
+        <v>33.095160999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8581,19 +8581,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>36.797150000000002</v>
+        <v>37.750587000000003</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>38.412365000000001</v>
+        <v>39.167709000000002</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>34.759304</v>
+        <v>33.323334000000003</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8601,19 +8601,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>30.933146000000001</v>
+        <v>32.999721999999998</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>21.073996999999999</v>
+        <v>22.779028</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>20.805440999999998</v>
+        <v>22.738938999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8621,19 +8621,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>31.153697999999999</v>
+        <v>32.989418000000001</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>26.352744999999999</v>
+        <v>27.471257999999999</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>25.39809</v>
+        <v>27.305260000000001</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8641,19 +8641,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>30.899647000000002</v>
+        <v>32.905132000000002</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>30.899647000000002</v>
+        <v>32.905132000000002</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>27.031410000000001</v>
+        <v>28.801749999999998</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8661,19 +8661,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>30.831762000000001</v>
+        <v>32.944232999999997</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>32.086844999999997</v>
+        <v>33.956333000000001</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>28.770468000000001</v>
+        <v>29.536162999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -8681,19 +8681,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>30.786688000000002</v>
+        <v>32.892417999999999</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>32.393700000000003</v>
+        <v>34.035122000000001</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>29.359988999999999</v>
+        <v>30.126584999999999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -8701,19 +8701,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>30.791183</v>
+        <v>32.676471999999997</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>32.549030000000002</v>
+        <v>34.061698999999997</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>29.705095</v>
+        <v>30.388870000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -8721,19 +8721,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>30.580539999999999</v>
+        <v>32.626807999999997</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>30.580539999999999</v>
+        <v>32.626807999999997</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>29.865494000000002</v>
+        <v>30.692335</v>
       </c>
     </row>
   </sheetData>
@@ -8747,7 +8747,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8788,19 +8788,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>29.850273000000001</v>
+        <v>32.881531000000003</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>33.456001000000001</v>
+        <v>34.352325</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>33.456001000000001</v>
+        <v>34.352325</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8808,19 +8808,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>29.829595999999999</v>
+        <v>32.986404</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>34.168976000000001</v>
+        <v>35.006332</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>34.168976000000001</v>
+        <v>35.006332</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8828,19 +8828,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>29.877098</v>
+        <v>32.931587</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>34.502116999999998</v>
+        <v>35.557068000000001</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>34.502116999999998</v>
+        <v>35.557068000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8848,19 +8848,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>29.718741999999999</v>
+        <v>32.914935999999997</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>29.718741999999999</v>
+        <v>32.914935999999997</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>34.494083000000003</v>
+        <v>35.637794</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8868,19 +8868,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>29.699404000000001</v>
+        <v>32.921638000000002</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>32.801926000000002</v>
+        <v>34.665264000000001</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>34.523617000000002</v>
+        <v>35.687389000000003</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8888,19 +8888,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>29.683685000000001</v>
+        <v>32.868858000000003</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>34.135883</v>
+        <v>35.458809000000002</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>35.091895999999998</v>
+        <v>35.914794999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8908,19 +8908,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>35.040691000000002</v>
+        <v>36.172652999999997</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>23.665482000000001</v>
+        <v>23.881233000000002</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>24.018940000000001</v>
+        <v>24.539190000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8928,19 +8928,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>35.052055000000003</v>
+        <v>36.181156000000001</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>35.052055000000003</v>
+        <v>36.181156000000001</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>30.361965000000001</v>
+        <v>28.903199999999998</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8948,19 +8948,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>35.014301000000003</v>
+        <v>36.166392999999999</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>37.925635999999997</v>
+        <v>38.439255000000003</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>32.183281000000001</v>
+        <v>33.032898000000003</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8968,19 +8968,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>35.010815000000001</v>
+        <v>36.141379999999998</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>39.509425999999998</v>
+        <v>39.893386999999997</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>34.727454999999999</v>
+        <v>34.301861000000002</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8988,19 +8988,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>35.026440000000001</v>
+        <v>36.221694999999997</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>40.210692999999999</v>
+        <v>40.327922999999998</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>35.920475000000003</v>
+        <v>34.770195000000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9008,19 +9008,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>35.042693999999997</v>
+        <v>36.197647000000003</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>35.042693999999997</v>
+        <v>36.197647000000003</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>36.406334000000001</v>
+        <v>35.139763000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9028,19 +9028,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>34.995995000000001</v>
+        <v>35.967609000000003</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>37.853518999999999</v>
+        <v>38.604725000000002</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>36.957703000000002</v>
+        <v>35.203026000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9048,19 +9048,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>29.619909</v>
+        <v>32.800026000000003</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>20.299306999999999</v>
+        <v>23.920334</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>21.222179000000001</v>
+        <v>23.242861000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9068,19 +9068,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>29.190318999999999</v>
+        <v>32.793658999999998</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>24.367775000000002</v>
+        <v>28.541819</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>26.213009</v>
+        <v>27.613441000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9088,19 +9088,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>29.182279999999999</v>
+        <v>32.833832000000001</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>29.182279999999999</v>
+        <v>32.833832000000001</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>28.358971</v>
+        <v>29.790945000000001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9108,19 +9108,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>29.235727000000001</v>
+        <v>32.843178000000002</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>32.058422</v>
+        <v>34.511825999999999</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>29.705147</v>
+        <v>30.262892000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9128,19 +9128,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>29.139481</v>
+        <v>32.300201000000001</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>32.7729</v>
+        <v>34.956394000000003</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>30.502040999999998</v>
+        <v>30.463058</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9148,19 +9148,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>29.256661999999999</v>
+        <v>32.285674999999998</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>33.134014000000001</v>
+        <v>34.556598999999999</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>30.806025999999999</v>
+        <v>31.125328</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9168,19 +9168,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>29.063071999999998</v>
+        <v>32.268013000000003</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>29.063071999999998</v>
+        <v>32.268013000000003</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>30.855761000000001</v>
+        <v>31.308893000000001</v>
       </c>
     </row>
   </sheetData>
@@ -9193,8 +9193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9312,7 +9312,7 @@
         <v>37467</v>
       </c>
       <c r="P4">
-        <v>78199</v>
+        <v>79228</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -9344,7 +9344,7 @@
         <v>35322</v>
       </c>
       <c r="P5">
-        <v>81695</v>
+        <v>83375</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -9376,7 +9376,7 @@
         <v>32589</v>
       </c>
       <c r="P6">
-        <v>81021</v>
+        <v>79187</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -9408,7 +9408,7 @@
         <v>33020</v>
       </c>
       <c r="P7">
-        <v>79009</v>
+        <v>83509</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -9440,7 +9440,7 @@
         <v>31872</v>
       </c>
       <c r="P8">
-        <v>81037</v>
+        <v>82348</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -9472,7 +9472,7 @@
         <v>30227</v>
       </c>
       <c r="P9">
-        <v>79972</v>
+        <v>78191</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -9504,7 +9504,7 @@
         <v>33008</v>
       </c>
       <c r="P10">
-        <v>80522</v>
+        <v>80028</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -9536,7 +9536,7 @@
         <v>24506</v>
       </c>
       <c r="P11">
-        <v>79832</v>
+        <v>80060</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -9568,7 +9568,7 @@
         <v>21377</v>
       </c>
       <c r="P12">
-        <v>81977</v>
+        <v>81075</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -9600,7 +9600,7 @@
         <v>19422</v>
       </c>
       <c r="P13">
-        <v>76938</v>
+        <v>83297</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -9632,7 +9632,7 @@
         <v>17176</v>
       </c>
       <c r="P14">
-        <v>81716</v>
+        <v>71991</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -9664,7 +9664,7 @@
         <v>17004</v>
       </c>
       <c r="P15">
-        <v>73925</v>
+        <v>77777</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -9696,7 +9696,7 @@
         <v>16459</v>
       </c>
       <c r="P16">
-        <v>82606</v>
+        <v>73438</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -9728,7 +9728,7 @@
         <v>34572</v>
       </c>
       <c r="P17">
-        <v>81339</v>
+        <v>80727</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -9760,7 +9760,7 @@
         <v>26665</v>
       </c>
       <c r="P18">
-        <v>80225</v>
+        <v>83899</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -9792,7 +9792,7 @@
         <v>25374</v>
       </c>
       <c r="P19">
-        <v>80798</v>
+        <v>84656</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -9824,7 +9824,7 @@
         <v>23234</v>
       </c>
       <c r="P20">
-        <v>84661</v>
+        <v>80427</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -9856,7 +9856,7 @@
         <v>23376</v>
       </c>
       <c r="P21">
-        <v>82641</v>
+        <v>82393</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -9888,7 +9888,7 @@
         <v>21917</v>
       </c>
       <c r="P22">
-        <v>81634</v>
+        <v>81979</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>23745</v>
       </c>
       <c r="P23">
-        <v>80497</v>
+        <v>85330</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -9982,37 +9982,37 @@
       </c>
       <c r="P24">
         <f t="shared" si="0"/>
-        <v>1691586</v>
+        <v>1694257</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25">
         <f>P24/B24</f>
-        <v>0.22468670648880548</v>
+        <v>0.22504148489973558</v>
       </c>
       <c r="C25">
         <f>P24/C24</f>
-        <v>0.32250091655000473</v>
+        <v>0.32301014277208573</v>
       </c>
       <c r="D25">
         <f>P24/D24</f>
-        <v>0.47168894817736273</v>
+        <v>0.47243374104073577</v>
       </c>
       <c r="E25">
         <f>P24/E24</f>
-        <v>0.7301550577986653</v>
+        <v>0.73130796646507668</v>
       </c>
       <c r="F25">
         <f>P24/F24</f>
-        <v>1.2090572834582356</v>
+        <v>1.2109663746922117</v>
       </c>
       <c r="G25">
         <f>P24/G24</f>
-        <v>1.9020283147750234</v>
+        <v>1.9050316014118034</v>
       </c>
       <c r="H25">
         <f>P24/H24</f>
-        <v>2.6355300939955346</v>
+        <v>2.6396915737435713</v>
       </c>
     </row>
   </sheetData>
@@ -10025,8 +10025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10061,7 +10061,7 @@
         <v>33.832417</v>
       </c>
       <c r="C3">
-        <v>32.792614</v>
+        <v>33.977221999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -10072,7 +10072,7 @@
         <v>33.763565</v>
       </c>
       <c r="C4">
-        <v>33.232483000000002</v>
+        <v>34.17915</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -10083,7 +10083,7 @@
         <v>33.776321000000003</v>
       </c>
       <c r="C5">
-        <v>33.418678</v>
+        <v>34.373299000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -10094,7 +10094,7 @@
         <v>33.721691</v>
       </c>
       <c r="C6">
-        <v>33.284270999999997</v>
+        <v>34.428963000000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -10105,7 +10105,7 @@
         <v>33.596901000000003</v>
       </c>
       <c r="C7">
-        <v>33.123874999999998</v>
+        <v>34.163581999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -10116,7 +10116,7 @@
         <v>33.680523000000001</v>
       </c>
       <c r="C8">
-        <v>33.753342000000004</v>
+        <v>34.500087999999998</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>28.603543999999999</v>
       </c>
       <c r="C9">
-        <v>22.994844000000001</v>
+        <v>23.703171000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -10138,7 +10138,7 @@
         <v>30.480953</v>
       </c>
       <c r="C10">
-        <v>29.168758</v>
+        <v>28.713322000000002</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -10149,7 +10149,7 @@
         <v>31.097985999999999</v>
       </c>
       <c r="C11">
-        <v>32.136276000000002</v>
+        <v>30.99127</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -10160,7 +10160,7 @@
         <v>31.399291999999999</v>
       </c>
       <c r="C12">
-        <v>33.205719000000002</v>
+        <v>32.092789000000003</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -10171,7 +10171,7 @@
         <v>31.589500000000001</v>
       </c>
       <c r="C13">
-        <v>34.017895000000003</v>
+        <v>32.687973</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -10182,7 +10182,7 @@
         <v>31.729956000000001</v>
       </c>
       <c r="C14">
-        <v>34.439681999999998</v>
+        <v>33.095160999999997</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -10193,7 +10193,7 @@
         <v>31.826536000000001</v>
       </c>
       <c r="C15">
-        <v>34.759304</v>
+        <v>33.323334000000003</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -10204,7 +10204,7 @@
         <v>28.317527999999999</v>
       </c>
       <c r="C16">
-        <v>20.805440999999998</v>
+        <v>22.738938999999998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>29.531122</v>
       </c>
       <c r="C17">
-        <v>25.39809</v>
+        <v>27.305260000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -10226,7 +10226,7 @@
         <v>29.914370999999999</v>
       </c>
       <c r="C18">
-        <v>27.031410000000001</v>
+        <v>28.801749999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -10237,7 +10237,7 @@
         <v>30.1511</v>
       </c>
       <c r="C19">
-        <v>28.770468000000001</v>
+        <v>29.536162999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -10248,7 +10248,7 @@
         <v>30.318769</v>
       </c>
       <c r="C20">
-        <v>29.359988999999999</v>
+        <v>30.126584999999999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -10259,7 +10259,7 @@
         <v>30.407647999999998</v>
       </c>
       <c r="C21">
-        <v>29.705095</v>
+        <v>30.388870000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -10270,7 +10270,7 @@
         <v>30.475828</v>
       </c>
       <c r="C22">
-        <v>29.865494000000002</v>
+        <v>30.692335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating exercise 1 data
</commit_message>
<xml_diff>
--- a/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
+++ b/goldendata/Assigment3_E1/BitcountAndPSNRGraphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CIF - bitcount" sheetId="1" r:id="rId1"/>
@@ -238,67 +238,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>81342</c:v>
+                  <c:v>81524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84595</c:v>
+                  <c:v>82527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80962</c:v>
+                  <c:v>83618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82299</c:v>
+                  <c:v>82203</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80978</c:v>
+                  <c:v>80734</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83020</c:v>
+                  <c:v>80762</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80925</c:v>
+                  <c:v>83760</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77491</c:v>
+                  <c:v>76932</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75549</c:v>
+                  <c:v>77313</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75578</c:v>
+                  <c:v>76893</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>77700</c:v>
+                  <c:v>76790</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>76962</c:v>
+                  <c:v>76505</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76412</c:v>
+                  <c:v>76416</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>76591</c:v>
+                  <c:v>76595</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>83125</c:v>
+                  <c:v>81955</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>82578</c:v>
+                  <c:v>84058</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>82174</c:v>
+                  <c:v>81613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>83413</c:v>
+                  <c:v>84170</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>83933</c:v>
+                  <c:v>82667</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>83668</c:v>
+                  <c:v>81232</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80411</c:v>
+                  <c:v>82911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,67 +355,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>81342</c:v>
+                  <c:v>81524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79228</c:v>
+                  <c:v>83325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83375</c:v>
+                  <c:v>81810</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79187</c:v>
+                  <c:v>81089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80978</c:v>
+                  <c:v>80734</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78584</c:v>
+                  <c:v>79189</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77552</c:v>
+                  <c:v>81146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80013</c:v>
+                  <c:v>85598</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75549</c:v>
+                  <c:v>77313</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>74458</c:v>
+                  <c:v>74491</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>68403</c:v>
+                  <c:v>73618</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64749</c:v>
+                  <c:v>64939</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76412</c:v>
+                  <c:v>76416</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73323</c:v>
+                  <c:v>76363</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>80796</c:v>
+                  <c:v>85524</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>81326</c:v>
+                  <c:v>81743</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>82174</c:v>
+                  <c:v>81613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>81990</c:v>
+                  <c:v>83596</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82465</c:v>
+                  <c:v>85688</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81220</c:v>
+                  <c:v>86799</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80411</c:v>
+                  <c:v>82911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -472,67 +472,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>81342</c:v>
+                  <c:v>81524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79228</c:v>
+                  <c:v>83325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83375</c:v>
+                  <c:v>81810</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79187</c:v>
+                  <c:v>81089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83509</c:v>
+                  <c:v>82940</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82348</c:v>
+                  <c:v>80535</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78191</c:v>
+                  <c:v>85019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80028</c:v>
+                  <c:v>85675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80060</c:v>
+                  <c:v>81952</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81075</c:v>
+                  <c:v>82766</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83297</c:v>
+                  <c:v>82222</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71991</c:v>
+                  <c:v>78872</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>77777</c:v>
+                  <c:v>80207</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73438</c:v>
+                  <c:v>71573</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>80727</c:v>
+                  <c:v>83747</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83899</c:v>
+                  <c:v>82772</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>84656</c:v>
+                  <c:v>88240</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80427</c:v>
+                  <c:v>86108</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82393</c:v>
+                  <c:v>80786</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81979</c:v>
+                  <c:v>81640</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>85330</c:v>
+                  <c:v>80726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,7 +666,8 @@
         <c:axId val="371746904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="60000"/>
+          <c:max val="100000"/>
+          <c:min val="50000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -991,67 +992,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>31324</c:v>
+                  <c:v>31372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30939</c:v>
+                  <c:v>30981</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31214</c:v>
+                  <c:v>31244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31400</c:v>
+                  <c:v>31426</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31764</c:v>
+                  <c:v>31805</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32130</c:v>
+                  <c:v>32192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31145</c:v>
+                  <c:v>31200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31572</c:v>
+                  <c:v>31615</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32031</c:v>
+                  <c:v>30290</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31875</c:v>
+                  <c:v>31918</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31905</c:v>
+                  <c:v>31948</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31700</c:v>
+                  <c:v>31743</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31855</c:v>
+                  <c:v>31898</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30134</c:v>
+                  <c:v>30177</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31725</c:v>
+                  <c:v>31779</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31970</c:v>
+                  <c:v>31944</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32078</c:v>
+                  <c:v>32050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32381</c:v>
+                  <c:v>32382</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31587</c:v>
+                  <c:v>31638</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31602</c:v>
+                  <c:v>31616</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32207</c:v>
+                  <c:v>32265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,67 +1109,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>31324</c:v>
+                  <c:v>31372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31977</c:v>
+                  <c:v>30715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31787</c:v>
+                  <c:v>32513</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32347</c:v>
+                  <c:v>33433</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31764</c:v>
+                  <c:v>31805</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30874</c:v>
+                  <c:v>31790</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30067</c:v>
+                  <c:v>30417</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32037</c:v>
+                  <c:v>32931</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32031</c:v>
+                  <c:v>30290</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27933</c:v>
+                  <c:v>32154</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29900</c:v>
+                  <c:v>30758</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24117</c:v>
+                  <c:v>27836</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31855</c:v>
+                  <c:v>31898</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28018</c:v>
+                  <c:v>29316</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32249</c:v>
+                  <c:v>33903</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33410</c:v>
+                  <c:v>32955</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32078</c:v>
+                  <c:v>32050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32671</c:v>
+                  <c:v>34923</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32300</c:v>
+                  <c:v>31597</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31386</c:v>
+                  <c:v>32691</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32207</c:v>
+                  <c:v>32265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1225,67 +1226,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>31324</c:v>
+                  <c:v>31372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31977</c:v>
+                  <c:v>30715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31787</c:v>
+                  <c:v>32513</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32347</c:v>
+                  <c:v>33433</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31369</c:v>
+                  <c:v>30774</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32987</c:v>
+                  <c:v>32757</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30597</c:v>
+                  <c:v>32743</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32213</c:v>
+                  <c:v>32864</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32296</c:v>
+                  <c:v>32689</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33528</c:v>
+                  <c:v>32968</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35328</c:v>
+                  <c:v>32631</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32199</c:v>
+                  <c:v>31176</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26898</c:v>
+                  <c:v>26791</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23635</c:v>
+                  <c:v>22505</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32362</c:v>
+                  <c:v>33730</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32362</c:v>
+                  <c:v>33063</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34667</c:v>
+                  <c:v>32712</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30961</c:v>
+                  <c:v>34654</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31734</c:v>
+                  <c:v>31291</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34462</c:v>
+                  <c:v>33439</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32727</c:v>
+                  <c:v>32281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,7 +1420,8 @@
         <c:axId val="371753176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="20000"/>
+          <c:max val="40000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1740,40 +1742,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>32.922676000000003</c:v>
+                  <c:v>33.209225000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.065178000000003</c:v>
+                  <c:v>33.317096999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.111407999999997</c:v>
+                  <c:v>33.416893000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.247089000000003</c:v>
+                  <c:v>33.455269000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.061886000000001</c:v>
+                  <c:v>33.281081999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.189579000000002</c:v>
+                  <c:v>33.240028000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.990250000000003</c:v>
+                  <c:v>33.317065999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.519649999999999</c:v>
+                  <c:v>37.653255000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.477913000000001</c:v>
+                  <c:v>37.681125999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.431870000000004</c:v>
+                  <c:v>37.654274000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.536411000000001</c:v>
+                  <c:v>37.669437000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>37.600158999999998</c:v>
+                  <c:v>37.726661999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>37.764488</c:v>
@@ -1782,25 +1784,25 @@
                   <c:v>37.750587000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.999721999999998</c:v>
+                  <c:v>33.185555000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32.989418000000001</c:v>
+                  <c:v>33.058132000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32.905132000000002</c:v>
+                  <c:v>33.026062000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.944232999999997</c:v>
+                  <c:v>33.071598000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.892417999999999</c:v>
+                  <c:v>32.905875999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.676471999999997</c:v>
+                  <c:v>32.733367999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.626807999999997</c:v>
+                  <c:v>32.800156000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1857,67 +1859,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>32.922676000000003</c:v>
+                  <c:v>33.209225000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.977221999999998</c:v>
+                  <c:v>34.483046999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.17915</c:v>
+                  <c:v>34.863140000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.373299000000003</c:v>
+                  <c:v>35.179104000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.061886000000001</c:v>
+                  <c:v>33.281081999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.032668999999999</c:v>
+                  <c:v>34.601542999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.421059</c:v>
+                  <c:v>35.082400999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.96011</c:v>
+                  <c:v>20.821190000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.477913000000001</c:v>
+                  <c:v>37.681125999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.012096</c:v>
+                  <c:v>39.673133999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.414776000000003</c:v>
+                  <c:v>40.277572999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39.556972999999999</c:v>
+                  <c:v>40.485027000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>37.764488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39.167709000000002</c:v>
+                  <c:v>39.799357999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.779028</c:v>
+                  <c:v>19.615508999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.471257999999999</c:v>
+                  <c:v>25.316632999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32.905132000000002</c:v>
+                  <c:v>33.026062000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.956333000000001</c:v>
+                  <c:v>34.251868999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.035122000000001</c:v>
+                  <c:v>34.579552</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.061698999999997</c:v>
+                  <c:v>34.611832</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.626807999999997</c:v>
+                  <c:v>32.800156000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,67 +1976,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>32.922676000000003</c:v>
+                  <c:v>33.209225000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.977221999999998</c:v>
+                  <c:v>34.483046999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.17915</c:v>
+                  <c:v>34.863140000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.373299000000003</c:v>
+                  <c:v>35.179104000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.428963000000003</c:v>
+                  <c:v>35.260593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.163581999999998</c:v>
+                  <c:v>34.979869999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.500087999999998</c:v>
+                  <c:v>35.361503999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.703171000000001</c:v>
+                  <c:v>20.756789999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.713322000000002</c:v>
+                  <c:v>26.126698000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.99127</c:v>
+                  <c:v>33.968029000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.092789000000003</c:v>
+                  <c:v>35.946967999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.687973</c:v>
+                  <c:v>36.622391</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33.095160999999997</c:v>
+                  <c:v>36.980365999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.323334000000003</c:v>
+                  <c:v>37.190429999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.738938999999998</c:v>
+                  <c:v>20.711213999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.305260000000001</c:v>
+                  <c:v>25.701533999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.801749999999998</c:v>
+                  <c:v>32.268374999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.536162999999998</c:v>
+                  <c:v>32.853240999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.126584999999999</c:v>
+                  <c:v>33.024704</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.388870000000001</c:v>
+                  <c:v>33.015647999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.692335</c:v>
+                  <c:v>32.982219999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2515,7 +2517,7 @@
                   <c:v>36.172652999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.181156000000001</c:v>
+                  <c:v>35.941177000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>36.166392999999999</c:v>
@@ -2611,61 +2613,61 @@
                   <c:v>32.892646999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.352325</c:v>
+                  <c:v>34.901854999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.006332</c:v>
+                  <c:v>36.121346000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.557068000000001</c:v>
+                  <c:v>36.705928999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>32.914935999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.665264000000001</c:v>
+                  <c:v>35.235160999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.458809000000002</c:v>
+                  <c:v>36.164538999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.881233000000002</c:v>
+                  <c:v>20.175901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.181156000000001</c:v>
+                  <c:v>35.941177000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.439255000000003</c:v>
+                  <c:v>38.579647000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.893386999999997</c:v>
+                  <c:v>40.258316000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.327922999999998</c:v>
+                  <c:v>40.766452999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>36.197647000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.604725000000002</c:v>
+                  <c:v>38.793564000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.920334</c:v>
+                  <c:v>19.261623</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.541819</c:v>
+                  <c:v>28.103034999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>32.833832000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34.511825999999999</c:v>
+                  <c:v>35.069954000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.956394000000003</c:v>
+                  <c:v>35.333832000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.556598999999999</c:v>
+                  <c:v>35.501949000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>32.268013000000003</c:v>
@@ -2728,64 +2730,64 @@
                   <c:v>32.892646999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.352325</c:v>
+                  <c:v>34.901854999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.006332</c:v>
+                  <c:v>36.121346000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.557068000000001</c:v>
+                  <c:v>36.705928999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.637794</c:v>
+                  <c:v>36.634377000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.687389000000003</c:v>
+                  <c:v>36.733952000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.914794999999998</c:v>
+                  <c:v>37.252952999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.539190000000001</c:v>
+                  <c:v>20.594902000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.903199999999998</c:v>
+                  <c:v>29.259143999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.032898000000003</c:v>
+                  <c:v>35.076293999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.301861000000002</c:v>
+                  <c:v>36.930515</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.770195000000001</c:v>
+                  <c:v>37.606681999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.139763000000002</c:v>
+                  <c:v>37.850676999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.203026000000001</c:v>
+                  <c:v>38.088645999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.242861000000001</c:v>
+                  <c:v>19.225525000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.613441000000002</c:v>
+                  <c:v>24.385054</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.790945000000001</c:v>
+                  <c:v>29.188337000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.262892000000001</c:v>
+                  <c:v>33.591358</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.463058</c:v>
+                  <c:v>33.780731000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31.125328</c:v>
+                  <c:v>33.748382999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31.308893000000001</c:v>
+                  <c:v>33.734763999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3220,67 +3222,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>81342</c:v>
+                  <c:v>81524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79228</c:v>
+                  <c:v>83325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83375</c:v>
+                  <c:v>81810</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79187</c:v>
+                  <c:v>81089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83509</c:v>
+                  <c:v>82940</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82348</c:v>
+                  <c:v>80535</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78191</c:v>
+                  <c:v>85019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80028</c:v>
+                  <c:v>85675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80060</c:v>
+                  <c:v>81952</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81075</c:v>
+                  <c:v>82766</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83297</c:v>
+                  <c:v>82222</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71991</c:v>
+                  <c:v>78872</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>77777</c:v>
+                  <c:v>80207</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73438</c:v>
+                  <c:v>71573</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>80727</c:v>
+                  <c:v>83747</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83899</c:v>
+                  <c:v>82772</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>84656</c:v>
+                  <c:v>88240</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80427</c:v>
+                  <c:v>86108</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82393</c:v>
+                  <c:v>80786</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81979</c:v>
+                  <c:v>81640</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>85330</c:v>
+                  <c:v>80726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3324,72 +3326,72 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Constant qp BitCount'!$F$3:$F$23</c:f>
+              <c:f>'Constant qp BitCount'!$E$3:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>83873</c:v>
+                  <c:v>141254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69603</c:v>
+                  <c:v>105334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64558</c:v>
+                  <c:v>98473</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59142</c:v>
+                  <c:v>91715</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64302</c:v>
+                  <c:v>97724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65438</c:v>
+                  <c:v>97256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53513</c:v>
+                  <c:v>81433</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>161619</c:v>
+                  <c:v>215548</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44083</c:v>
+                  <c:v>62364</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32142</c:v>
+                  <c:v>46443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27760</c:v>
+                  <c:v>40788</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25489</c:v>
+                  <c:v>40053</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23290</c:v>
+                  <c:v>39462</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21426</c:v>
+                  <c:v>37070</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>176026</c:v>
+                  <c:v>219219</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>82512</c:v>
+                  <c:v>122341</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74467</c:v>
+                  <c:v>116305</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>68746</c:v>
+                  <c:v>112679</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>67903</c:v>
+                  <c:v>116700</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>65891</c:v>
+                  <c:v>117471</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>67312</c:v>
+                  <c:v>120901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3818,67 +3820,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>32.922676000000003</c:v>
+                  <c:v>33.209225000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.977221999999998</c:v>
+                  <c:v>34.483046999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.17915</c:v>
+                  <c:v>34.863140000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.373299000000003</c:v>
+                  <c:v>35.179104000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.428963000000003</c:v>
+                  <c:v>35.260593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.163581999999998</c:v>
+                  <c:v>34.979869999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.500087999999998</c:v>
+                  <c:v>35.361503999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.703171000000001</c:v>
+                  <c:v>20.756789999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.713322000000002</c:v>
+                  <c:v>26.126698000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.99127</c:v>
+                  <c:v>33.968029000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.092789000000003</c:v>
+                  <c:v>35.946967999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.687973</c:v>
+                  <c:v>36.622391</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33.095160999999997</c:v>
+                  <c:v>36.980365999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.323334000000003</c:v>
+                  <c:v>37.190429999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.738938999999998</c:v>
+                  <c:v>20.711213999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.305260000000001</c:v>
+                  <c:v>25.701533999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.801749999999998</c:v>
+                  <c:v>32.268374999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.536162999999998</c:v>
+                  <c:v>32.853240999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.126584999999999</c:v>
+                  <c:v>33.024704</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.388870000000001</c:v>
+                  <c:v>33.015647999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.692335</c:v>
+                  <c:v>32.982219999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3927,67 +3929,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>33.654021999999998</c:v>
+                  <c:v>36.541454000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.832417</c:v>
+                  <c:v>36.826805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.763565</c:v>
+                  <c:v>36.802345000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.776321000000003</c:v>
+                  <c:v>36.866942999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.721691</c:v>
+                  <c:v>36.864071000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.596901000000003</c:v>
+                  <c:v>36.697563000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.680523000000001</c:v>
+                  <c:v>36.822231000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.603543999999999</c:v>
+                  <c:v>35.770888999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.480953</c:v>
+                  <c:v>36.497013000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.097985999999999</c:v>
+                  <c:v>36.860461999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.399291999999999</c:v>
+                  <c:v>37.069180000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.589500000000001</c:v>
+                  <c:v>37.168762000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.729956000000001</c:v>
+                  <c:v>37.284050000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31.826536000000001</c:v>
+                  <c:v>37.350613000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28.317527999999999</c:v>
+                  <c:v>34.898707999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.531122</c:v>
+                  <c:v>35.442383</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.914370999999999</c:v>
+                  <c:v>35.476542999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.1511</c:v>
+                  <c:v>35.541428000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.318769</c:v>
+                  <c:v>35.565033</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.407647999999998</c:v>
+                  <c:v>35.543807999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30.475828</c:v>
+                  <c:v>35.510756999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7737,15 +7739,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>81915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>17144</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>140969</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>150495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8119,7 +8121,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F22"/>
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8140,19 +8142,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>81342</v>
+        <v>81524</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>81342</v>
+        <v>81524</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>81342</v>
+        <v>81524</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8160,19 +8162,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>84595</v>
+        <v>82527</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>79228</v>
+        <v>83325</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>79228</v>
+        <v>83325</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8180,19 +8182,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>80962</v>
+        <v>83618</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>83375</v>
+        <v>81810</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>83375</v>
+        <v>81810</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8200,19 +8202,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>82299</v>
+        <v>82203</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>79187</v>
+        <v>81089</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>79187</v>
+        <v>81089</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8220,19 +8222,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>80978</v>
+        <v>80734</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>80978</v>
+        <v>80734</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>83509</v>
+        <v>82940</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8240,19 +8242,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>83020</v>
+        <v>80762</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>78584</v>
+        <v>79189</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>82348</v>
+        <v>80535</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8260,19 +8262,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>80925</v>
+        <v>83760</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>77552</v>
+        <v>81146</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>78191</v>
+        <v>85019</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8280,19 +8282,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>77491</v>
+        <v>76932</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>80013</v>
+        <v>85598</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>80028</v>
+        <v>85675</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8300,19 +8302,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>75549</v>
+        <v>77313</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>75549</v>
+        <v>77313</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>80060</v>
+        <v>81952</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8320,19 +8322,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>75578</v>
+        <v>76893</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>74458</v>
+        <v>74491</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>81075</v>
+        <v>82766</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8340,19 +8342,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>77700</v>
+        <v>76790</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>68403</v>
+        <v>73618</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>83297</v>
+        <v>82222</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8360,19 +8362,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>76962</v>
+        <v>76505</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>64749</v>
+        <v>64939</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>71991</v>
+        <v>78872</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8380,19 +8382,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>76412</v>
+        <v>76416</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>76412</v>
+        <v>76416</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>77777</v>
+        <v>80207</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8400,19 +8402,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>76591</v>
+        <v>76595</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>73323</v>
+        <v>76363</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>73438</v>
+        <v>71573</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8420,19 +8422,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>83125</v>
+        <v>81955</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>80796</v>
+        <v>85524</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>80727</v>
+        <v>83747</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8440,19 +8442,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82578</v>
+        <v>84058</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>81326</v>
+        <v>81743</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>83899</v>
+        <v>82772</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8460,19 +8462,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>82174</v>
+        <v>81613</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>82174</v>
+        <v>81613</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>84656</v>
+        <v>88240</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8480,19 +8482,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>83413</v>
+        <v>84170</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>81990</v>
+        <v>83596</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>80427</v>
+        <v>86108</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -8500,19 +8502,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>83933</v>
+        <v>82667</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>82465</v>
+        <v>85688</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>82393</v>
+        <v>80786</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -8520,19 +8522,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>83668</v>
+        <v>81232</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>81220</v>
+        <v>86799</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>81979</v>
+        <v>81640</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -8540,19 +8542,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>80411</v>
+        <v>82911</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>80411</v>
+        <v>82911</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>85330</v>
+        <v>80726</v>
       </c>
     </row>
   </sheetData>
@@ -8565,8 +8567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8587,19 +8589,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>31324</v>
+        <v>31372</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>31324</v>
+        <v>31372</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>31324</v>
+        <v>31372</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8607,19 +8609,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>30939</v>
+        <v>30981</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>31977</v>
+        <v>30715</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>31977</v>
+        <v>30715</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8627,19 +8629,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>31214</v>
+        <v>31244</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>31787</v>
+        <v>32513</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>31787</v>
+        <v>32513</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8647,19 +8649,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>31400</v>
+        <v>31426</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>32347</v>
+        <v>33433</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>32347</v>
+        <v>33433</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8667,19 +8669,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>31764</v>
+        <v>31805</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>31764</v>
+        <v>31805</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>31369</v>
+        <v>30774</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8687,19 +8689,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>32130</v>
+        <v>32192</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>30874</v>
+        <v>31790</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>32987</v>
+        <v>32757</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8707,19 +8709,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>31145</v>
+        <v>31200</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>30067</v>
+        <v>30417</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>30597</v>
+        <v>32743</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8727,19 +8729,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>31572</v>
+        <v>31615</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>32037</v>
+        <v>32931</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>32213</v>
+        <v>32864</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8747,19 +8749,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>32031</v>
+        <v>30290</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>32031</v>
+        <v>30290</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>32296</v>
+        <v>32689</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8767,19 +8769,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>31875</v>
+        <v>31918</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>27933</v>
+        <v>32154</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>33528</v>
+        <v>32968</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8787,19 +8789,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>31905</v>
+        <v>31948</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>29900</v>
+        <v>30758</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>35328</v>
+        <v>32631</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8807,19 +8809,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>31700</v>
+        <v>31743</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>24117</v>
+        <v>27836</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>32199</v>
+        <v>31176</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8827,19 +8829,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>31855</v>
+        <v>31898</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>31855</v>
+        <v>31898</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>26898</v>
+        <v>26791</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8847,19 +8849,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>30134</v>
+        <v>30177</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>28018</v>
+        <v>29316</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>23635</v>
+        <v>22505</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8867,19 +8869,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>31725</v>
+        <v>31779</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>32249</v>
+        <v>33903</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>32362</v>
+        <v>33730</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8887,19 +8889,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>31970</v>
+        <v>31944</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>33410</v>
+        <v>32955</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>32362</v>
+        <v>33063</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8907,19 +8909,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>32078</v>
+        <v>32050</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>32078</v>
+        <v>32050</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>34667</v>
+        <v>32712</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8927,19 +8929,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>32381</v>
+        <v>32382</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>32671</v>
+        <v>34923</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>30961</v>
+        <v>34654</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -8947,19 +8949,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>31587</v>
+        <v>31638</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>32300</v>
+        <v>31597</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>31734</v>
+        <v>31291</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -8967,19 +8969,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>31602</v>
+        <v>31616</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>31386</v>
+        <v>32691</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>34462</v>
+        <v>33439</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -8987,19 +8989,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>32207</v>
+        <v>32265</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>32207</v>
+        <v>32265</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>32727</v>
+        <v>32281</v>
       </c>
     </row>
   </sheetData>
@@ -9013,7 +9015,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F22"/>
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9034,19 +9036,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>32.922676000000003</v>
+        <v>33.209225000000004</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>32.922676000000003</v>
+        <v>33.209225000000004</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>32.922676000000003</v>
+        <v>33.209225000000004</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9054,19 +9056,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>33.065178000000003</v>
+        <v>33.317096999999997</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>33.977221999999998</v>
+        <v>34.483046999999999</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>33.977221999999998</v>
+        <v>34.483046999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9074,19 +9076,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>33.111407999999997</v>
+        <v>33.416893000000002</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>34.17915</v>
+        <v>34.863140000000001</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>34.17915</v>
+        <v>34.863140000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9094,19 +9096,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>33.247089000000003</v>
+        <v>33.455269000000001</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>34.373299000000003</v>
+        <v>35.179104000000002</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>34.373299000000003</v>
+        <v>35.179104000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9114,19 +9116,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>33.061886000000001</v>
+        <v>33.281081999999998</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>33.061886000000001</v>
+        <v>33.281081999999998</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>34.428963000000003</v>
+        <v>35.260593</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9134,19 +9136,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>33.189579000000002</v>
+        <v>33.240028000000002</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>34.032668999999999</v>
+        <v>34.601542999999999</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>34.163581999999998</v>
+        <v>34.979869999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9154,19 +9156,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>32.990250000000003</v>
+        <v>33.317065999999997</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>34.421059</v>
+        <v>35.082400999999997</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>34.500087999999998</v>
+        <v>35.361503999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9174,19 +9176,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>37.519649999999999</v>
+        <v>37.653255000000001</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>23.96011</v>
+        <v>20.821190000000001</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>23.703171000000001</v>
+        <v>20.756789999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9194,19 +9196,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>37.477913000000001</v>
+        <v>37.681125999999999</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>37.477913000000001</v>
+        <v>37.681125999999999</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>28.713322000000002</v>
+        <v>26.126698000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9214,19 +9216,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>37.431870000000004</v>
+        <v>37.654274000000001</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>39.012096</v>
+        <v>39.673133999999997</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>30.99127</v>
+        <v>33.968029000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9234,19 +9236,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>37.536411000000001</v>
+        <v>37.669437000000002</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>39.414776000000003</v>
+        <v>40.277572999999997</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>32.092789000000003</v>
+        <v>35.946967999999998</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9254,19 +9256,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>37.600158999999998</v>
+        <v>37.726661999999997</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>39.556972999999999</v>
+        <v>40.485027000000002</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>32.687973</v>
+        <v>36.622391</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9286,7 +9288,7 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>33.095160999999997</v>
+        <v>36.980365999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9300,13 +9302,13 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>39.167709000000002</v>
+        <v>39.799357999999998</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>33.323334000000003</v>
+        <v>37.190429999999999</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9314,19 +9316,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>32.999721999999998</v>
+        <v>33.185555000000001</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>22.779028</v>
+        <v>19.615508999999999</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>22.738938999999998</v>
+        <v>20.711213999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9334,19 +9336,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>32.989418000000001</v>
+        <v>33.058132000000001</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>27.471257999999999</v>
+        <v>25.316632999999999</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>27.305260000000001</v>
+        <v>25.701533999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9354,19 +9356,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>32.905132000000002</v>
+        <v>33.026062000000003</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>32.905132000000002</v>
+        <v>33.026062000000003</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>28.801749999999998</v>
+        <v>32.268374999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9374,19 +9376,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>32.944232999999997</v>
+        <v>33.071598000000002</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>33.956333000000001</v>
+        <v>34.251868999999999</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>29.536162999999998</v>
+        <v>32.853240999999997</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9394,19 +9396,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>32.892417999999999</v>
+        <v>32.905875999999999</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>34.035122000000001</v>
+        <v>34.579552</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>30.126584999999999</v>
+        <v>33.024704</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9414,19 +9416,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>32.676471999999997</v>
+        <v>32.733367999999999</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21">
-        <v>34.061698999999997</v>
+        <v>34.611832</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>30.388870000000001</v>
+        <v>33.015647999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9434,19 +9436,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>32.626807999999997</v>
+        <v>32.800156000000001</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22">
-        <v>32.626807999999997</v>
+        <v>32.800156000000001</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>30.692335</v>
+        <v>32.982219999999998</v>
       </c>
     </row>
   </sheetData>
@@ -9460,7 +9462,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F22"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,13 +9509,13 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>34.352325</v>
+        <v>34.901854999999998</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>34.352325</v>
+        <v>34.901854999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9527,13 +9529,13 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>35.006332</v>
+        <v>36.121346000000003</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>35.006332</v>
+        <v>36.121346000000003</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9547,13 +9549,13 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>35.557068000000001</v>
+        <v>36.705928999999998</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>35.557068000000001</v>
+        <v>36.705928999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9573,7 +9575,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>35.637794</v>
+        <v>36.634377000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9587,13 +9589,13 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>34.665264000000001</v>
+        <v>35.235160999999998</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>35.687389000000003</v>
+        <v>36.733952000000002</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9607,13 +9609,13 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>35.458809000000002</v>
+        <v>36.164538999999998</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>35.914794999999998</v>
+        <v>37.252952999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9627,13 +9629,13 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>23.881233000000002</v>
+        <v>20.175901</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>24.539190000000001</v>
+        <v>20.594902000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9641,19 +9643,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>36.181156000000001</v>
+        <v>35.941177000000003</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>36.181156000000001</v>
+        <v>35.941177000000003</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>28.903199999999998</v>
+        <v>29.259143999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9667,13 +9669,13 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>38.439255000000003</v>
+        <v>38.579647000000001</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>33.032898000000003</v>
+        <v>35.076293999999997</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9687,13 +9689,13 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>39.893386999999997</v>
+        <v>40.258316000000001</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>34.301861000000002</v>
+        <v>36.930515</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9707,13 +9709,13 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>40.327922999999998</v>
+        <v>40.766452999999998</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>34.770195000000001</v>
+        <v>37.606681999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9733,7 +9735,7 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>35.139763000000002</v>
+        <v>37.850676999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9747,13 +9749,13 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>38.604725000000002</v>
+        <v>38.793564000000003</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>35.203026000000001</v>
+        <v>38.088645999999997</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9767,13 +9769,13 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>23.920334</v>
+        <v>19.261623</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>23.242861000000001</v>
+        <v>19.225525000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9787,13 +9789,13 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>28.541819</v>
+        <v>28.103034999999998</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>27.613441000000002</v>
+        <v>24.385054</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9813,7 +9815,7 @@
         <v>16</v>
       </c>
       <c r="F18">
-        <v>29.790945000000001</v>
+        <v>29.188337000000001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9827,13 +9829,13 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>34.511825999999999</v>
+        <v>35.069954000000003</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>30.262892000000001</v>
+        <v>33.591358</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9847,13 +9849,13 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>34.956394000000003</v>
+        <v>35.333832000000001</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20">
-        <v>30.463058</v>
+        <v>33.780731000000003</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9867,13 +9869,13 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>34.556598999999999</v>
+        <v>35.501949000000003</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21">
-        <v>31.125328</v>
+        <v>33.748382999999997</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9893,7 +9895,7 @@
         <v>20</v>
       </c>
       <c r="F22">
-        <v>31.308893000000001</v>
+        <v>33.734763999999998</v>
       </c>
     </row>
   </sheetData>
@@ -9906,8 +9908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9968,709 +9970,307 @@
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>437383</v>
-      </c>
-      <c r="C3">
-        <v>316806</v>
-      </c>
-      <c r="D3">
-        <v>220803</v>
-      </c>
       <c r="E3">
-        <v>141238</v>
+        <v>141254</v>
       </c>
       <c r="F3">
-        <v>83873</v>
-      </c>
-      <c r="G3">
-        <v>50332</v>
-      </c>
-      <c r="H3">
-        <v>31719</v>
-      </c>
-      <c r="I3">
-        <v>21820</v>
+        <v>83903</v>
       </c>
       <c r="P3">
-        <v>81342</v>
+        <v>81524</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>405329</v>
-      </c>
-      <c r="C4">
-        <v>286482</v>
-      </c>
-      <c r="D4">
-        <v>195337</v>
-      </c>
       <c r="E4">
-        <v>126466</v>
+        <v>105334</v>
       </c>
       <c r="F4">
-        <v>69603</v>
-      </c>
-      <c r="G4">
-        <v>49151</v>
-      </c>
-      <c r="H4">
-        <v>39783</v>
-      </c>
-      <c r="I4">
-        <v>37467</v>
+        <v>59482</v>
       </c>
       <c r="P4">
-        <v>79228</v>
+        <v>83325</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>400378</v>
-      </c>
-      <c r="C5">
-        <v>283820</v>
-      </c>
-      <c r="D5">
-        <v>188992</v>
-      </c>
       <c r="E5">
-        <v>115737</v>
+        <v>98473</v>
       </c>
       <c r="F5">
-        <v>64558</v>
-      </c>
-      <c r="G5">
-        <v>43637</v>
-      </c>
-      <c r="H5">
-        <v>35110</v>
-      </c>
-      <c r="I5">
-        <v>35322</v>
+        <v>53449</v>
       </c>
       <c r="P5">
-        <v>83375</v>
+        <v>81810</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>381247</v>
-      </c>
-      <c r="C6">
-        <v>265941</v>
-      </c>
-      <c r="D6">
-        <v>176791</v>
-      </c>
       <c r="E6">
-        <v>104249</v>
+        <v>91715</v>
       </c>
       <c r="F6">
-        <v>59142</v>
-      </c>
-      <c r="G6">
-        <v>38760</v>
-      </c>
-      <c r="H6">
-        <v>33336</v>
-      </c>
-      <c r="I6">
-        <v>32589</v>
+        <v>47518</v>
       </c>
       <c r="P6">
-        <v>79187</v>
+        <v>81089</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>404870</v>
-      </c>
-      <c r="C7">
-        <v>280502</v>
-      </c>
-      <c r="D7">
-        <v>188152</v>
-      </c>
       <c r="E7">
-        <v>114378</v>
+        <v>97724</v>
       </c>
       <c r="F7">
-        <v>64302</v>
-      </c>
-      <c r="G7">
-        <v>39236</v>
-      </c>
-      <c r="H7">
-        <v>31801</v>
-      </c>
-      <c r="I7">
-        <v>33020</v>
+        <v>50026</v>
       </c>
       <c r="P7">
-        <v>83509</v>
+        <v>82940</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>404423</v>
-      </c>
-      <c r="C8">
-        <v>281611</v>
-      </c>
-      <c r="D8">
-        <v>191837</v>
-      </c>
       <c r="E8">
-        <v>116837</v>
+        <v>97256</v>
       </c>
       <c r="F8">
-        <v>65438</v>
-      </c>
-      <c r="G8">
-        <v>38231</v>
-      </c>
-      <c r="H8">
-        <v>32211</v>
-      </c>
-      <c r="I8">
-        <v>31872</v>
+        <v>52165</v>
       </c>
       <c r="P8">
-        <v>82348</v>
+        <v>80535</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>351232</v>
-      </c>
-      <c r="C9">
-        <v>237979</v>
-      </c>
-      <c r="D9">
-        <v>152594</v>
-      </c>
       <c r="E9">
-        <v>92309</v>
+        <v>81433</v>
       </c>
       <c r="F9">
-        <v>53513</v>
-      </c>
-      <c r="G9">
-        <v>37562</v>
-      </c>
-      <c r="H9">
-        <v>30008</v>
-      </c>
-      <c r="I9">
-        <v>30227</v>
+        <v>45079</v>
       </c>
       <c r="P9">
-        <v>78191</v>
+        <v>85019</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>585636</v>
-      </c>
-      <c r="C10">
-        <v>443583</v>
-      </c>
-      <c r="D10">
-        <v>326211</v>
-      </c>
       <c r="E10">
-        <v>236491</v>
+        <v>215548</v>
       </c>
       <c r="F10">
-        <v>161619</v>
-      </c>
-      <c r="G10">
-        <v>99147</v>
-      </c>
-      <c r="H10">
-        <v>55450</v>
-      </c>
-      <c r="I10">
-        <v>33008</v>
+        <v>144573</v>
       </c>
       <c r="P10">
-        <v>80028</v>
+        <v>85675</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>199259</v>
-      </c>
-      <c r="C11">
-        <v>131883</v>
-      </c>
-      <c r="D11">
-        <v>97366</v>
-      </c>
       <c r="E11">
-        <v>63914</v>
+        <v>62364</v>
       </c>
       <c r="F11">
-        <v>44083</v>
-      </c>
-      <c r="G11">
-        <v>33513</v>
-      </c>
-      <c r="H11">
-        <v>28803</v>
-      </c>
-      <c r="I11">
-        <v>24506</v>
+        <v>40597</v>
       </c>
       <c r="P11">
-        <v>80060</v>
+        <v>81952</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12">
-        <v>163785</v>
-      </c>
-      <c r="C12">
-        <v>95979</v>
-      </c>
-      <c r="D12">
-        <v>66039</v>
-      </c>
       <c r="E12">
-        <v>43474</v>
+        <v>46443</v>
       </c>
       <c r="F12">
-        <v>32142</v>
-      </c>
-      <c r="G12">
-        <v>25783</v>
-      </c>
-      <c r="H12">
-        <v>23750</v>
-      </c>
-      <c r="I12">
-        <v>21377</v>
+        <v>33020</v>
       </c>
       <c r="P12">
-        <v>81075</v>
+        <v>82766</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>153023</v>
-      </c>
-      <c r="C13">
-        <v>82899</v>
-      </c>
-      <c r="D13">
-        <v>52984</v>
-      </c>
       <c r="E13">
-        <v>37430</v>
+        <v>40788</v>
       </c>
       <c r="F13">
-        <v>27760</v>
-      </c>
-      <c r="G13">
-        <v>23758</v>
-      </c>
-      <c r="H13">
-        <v>20918</v>
-      </c>
-      <c r="I13">
-        <v>19422</v>
+        <v>31159</v>
       </c>
       <c r="P13">
-        <v>83297</v>
+        <v>82222</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>151808</v>
-      </c>
-      <c r="C14">
-        <v>80689</v>
-      </c>
-      <c r="D14">
-        <v>49580</v>
-      </c>
       <c r="E14">
-        <v>35897</v>
+        <v>40053</v>
       </c>
       <c r="F14">
-        <v>25489</v>
-      </c>
-      <c r="G14">
-        <v>22162</v>
-      </c>
-      <c r="H14">
-        <v>19270</v>
-      </c>
-      <c r="I14">
-        <v>17176</v>
+        <v>30320</v>
       </c>
       <c r="P14">
-        <v>71991</v>
+        <v>78872</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>145457</v>
-      </c>
-      <c r="C15">
-        <v>75891</v>
-      </c>
-      <c r="D15">
-        <v>42928</v>
-      </c>
       <c r="E15">
-        <v>30958</v>
+        <v>39462</v>
       </c>
       <c r="F15">
-        <v>23290</v>
-      </c>
-      <c r="G15">
-        <v>19398</v>
-      </c>
-      <c r="H15">
-        <v>17123</v>
-      </c>
-      <c r="I15">
-        <v>17004</v>
+        <v>30151</v>
       </c>
       <c r="P15">
-        <v>77777</v>
+        <v>80207</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>146647</v>
-      </c>
-      <c r="C16">
-        <v>74525</v>
-      </c>
-      <c r="D16">
-        <v>42069</v>
-      </c>
       <c r="E16">
-        <v>27722</v>
+        <v>37070</v>
       </c>
       <c r="F16">
-        <v>21426</v>
-      </c>
-      <c r="G16">
-        <v>18565</v>
-      </c>
-      <c r="H16">
-        <v>16255</v>
-      </c>
-      <c r="I16">
-        <v>16459</v>
+        <v>29050</v>
       </c>
       <c r="P16">
-        <v>73438</v>
+        <v>71573</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>635621</v>
-      </c>
-      <c r="C17">
-        <v>485238</v>
-      </c>
-      <c r="D17">
-        <v>356936</v>
-      </c>
       <c r="E17">
-        <v>257443</v>
+        <v>219219</v>
       </c>
       <c r="F17">
-        <v>176026</v>
-      </c>
-      <c r="G17">
-        <v>107330</v>
-      </c>
-      <c r="H17">
-        <v>58451</v>
-      </c>
-      <c r="I17">
-        <v>34572</v>
+        <v>144110</v>
       </c>
       <c r="P17">
-        <v>80727</v>
+        <v>83747</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>428841</v>
-      </c>
-      <c r="C18">
-        <v>310415</v>
-      </c>
-      <c r="D18">
-        <v>218245</v>
-      </c>
       <c r="E18">
-        <v>143184</v>
+        <v>122341</v>
       </c>
       <c r="F18">
-        <v>82512</v>
-      </c>
-      <c r="G18">
-        <v>48008</v>
-      </c>
-      <c r="H18">
-        <v>31846</v>
-      </c>
-      <c r="I18">
-        <v>26665</v>
+        <v>68919</v>
       </c>
       <c r="P18">
-        <v>83899</v>
+        <v>82772</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19">
-        <v>431949</v>
-      </c>
-      <c r="C19">
-        <v>308809</v>
-      </c>
-      <c r="D19">
-        <v>211765</v>
-      </c>
       <c r="E19">
-        <v>131762</v>
+        <v>116305</v>
       </c>
       <c r="F19">
-        <v>74467</v>
-      </c>
-      <c r="G19">
-        <v>42582</v>
-      </c>
-      <c r="H19">
-        <v>28672</v>
-      </c>
-      <c r="I19">
-        <v>25374</v>
+        <v>62691</v>
       </c>
       <c r="P19">
-        <v>84656</v>
+        <v>88240</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>422521</v>
-      </c>
-      <c r="C20">
-        <v>301904</v>
-      </c>
-      <c r="D20">
-        <v>204743</v>
-      </c>
       <c r="E20">
-        <v>124552</v>
+        <v>112679</v>
       </c>
       <c r="F20">
-        <v>68746</v>
-      </c>
-      <c r="G20">
-        <v>37557</v>
-      </c>
-      <c r="H20">
-        <v>27208</v>
-      </c>
-      <c r="I20">
-        <v>23234</v>
+        <v>62883</v>
       </c>
       <c r="P20">
-        <v>80427</v>
+        <v>86108</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>424918</v>
-      </c>
-      <c r="C21">
-        <v>298756</v>
-      </c>
-      <c r="D21">
-        <v>200171</v>
-      </c>
       <c r="E21">
-        <v>126486</v>
+        <v>116700</v>
       </c>
       <c r="F21">
-        <v>67903</v>
-      </c>
-      <c r="G21">
-        <v>38392</v>
-      </c>
-      <c r="H21">
-        <v>26629</v>
-      </c>
-      <c r="I21">
-        <v>23376</v>
+        <v>60007</v>
       </c>
       <c r="P21">
-        <v>82393</v>
+        <v>80786</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22">
-        <v>422774</v>
-      </c>
-      <c r="C22">
-        <v>299169</v>
-      </c>
-      <c r="D22">
-        <v>200113</v>
-      </c>
       <c r="E22">
-        <v>122565</v>
+        <v>117471</v>
       </c>
       <c r="F22">
-        <v>65891</v>
-      </c>
-      <c r="G22">
-        <v>38226</v>
-      </c>
-      <c r="H22">
-        <v>26597</v>
-      </c>
-      <c r="I22">
-        <v>21917</v>
+        <v>64820</v>
       </c>
       <c r="P22">
-        <v>81979</v>
+        <v>81640</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23">
-        <v>431542</v>
-      </c>
-      <c r="C23">
-        <v>302332</v>
-      </c>
-      <c r="D23">
-        <v>202576</v>
-      </c>
       <c r="E23">
-        <v>123657</v>
+        <v>120901</v>
       </c>
       <c r="F23">
-        <v>67312</v>
-      </c>
-      <c r="G23">
-        <v>38029</v>
-      </c>
-      <c r="H23">
-        <v>26899</v>
-      </c>
-      <c r="I23">
-        <v>23745</v>
+        <v>66290</v>
       </c>
       <c r="P23">
-        <v>85330</v>
+        <v>80726</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <f>SUM(B3:B23)</f>
-        <v>7528643</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:P24" si="0">SUM(C3:C23)</f>
-        <v>5245213</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>3586232</v>
-      </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>2316749</v>
+        <f>SUM(E2:E23)</f>
+        <v>2120536</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>1399095</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>889359</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>641839</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>550152</v>
+        <f>SUM(F3:F23)</f>
+        <v>1260212</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J24:P24" si="0">SUM(J3:J23)</f>
         <v>0</v>
       </c>
       <c r="K24">
@@ -10695,37 +10295,17 @@
       </c>
       <c r="P24">
         <f t="shared" si="0"/>
-        <v>1694257</v>
+        <v>1723528</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <f>P24/B24</f>
-        <v>0.22504148489973558</v>
-      </c>
-      <c r="C25">
-        <f>P24/C24</f>
-        <v>0.32301014277208573</v>
-      </c>
-      <c r="D25">
-        <f>P24/D24</f>
-        <v>0.47243374104073577</v>
-      </c>
       <c r="E25">
         <f>P24/E24</f>
-        <v>0.73130796646507668</v>
+        <v>0.81277941048866886</v>
       </c>
       <c r="F25">
         <f>P24/F24</f>
-        <v>1.2109663746922117</v>
-      </c>
-      <c r="G25">
-        <f>P24/G24</f>
-        <v>1.9050316014118034</v>
-      </c>
-      <c r="H25">
-        <f>P24/H24</f>
-        <v>2.6396915737435713</v>
+        <v>1.3676492526654245</v>
       </c>
     </row>
   </sheetData>
@@ -10739,7 +10319,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C22"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10760,10 +10340,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>33.654021999999998</v>
+        <v>36.541454000000002</v>
       </c>
       <c r="C2">
-        <v>32.922676000000003</v>
+        <v>33.209225000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -10771,10 +10351,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>33.832417</v>
+        <v>36.826805</v>
       </c>
       <c r="C3">
-        <v>33.977221999999998</v>
+        <v>34.483046999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -10782,10 +10362,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>33.763565</v>
+        <v>36.802345000000003</v>
       </c>
       <c r="C4">
-        <v>34.17915</v>
+        <v>34.863140000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -10793,10 +10373,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>33.776321000000003</v>
+        <v>36.866942999999999</v>
       </c>
       <c r="C5">
-        <v>34.373299000000003</v>
+        <v>35.179104000000002</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -10804,10 +10384,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>33.721691</v>
+        <v>36.864071000000003</v>
       </c>
       <c r="C6">
-        <v>34.428963000000003</v>
+        <v>35.260593</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -10815,10 +10395,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>33.596901000000003</v>
+        <v>36.697563000000002</v>
       </c>
       <c r="C7">
-        <v>34.163581999999998</v>
+        <v>34.979869999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -10826,10 +10406,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>33.680523000000001</v>
+        <v>36.822231000000002</v>
       </c>
       <c r="C8">
-        <v>34.500087999999998</v>
+        <v>35.361503999999996</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -10837,10 +10417,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>28.603543999999999</v>
+        <v>35.770888999999997</v>
       </c>
       <c r="C9">
-        <v>23.703171000000001</v>
+        <v>20.756789999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -10848,10 +10428,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>30.480953</v>
+        <v>36.497013000000003</v>
       </c>
       <c r="C10">
-        <v>28.713322000000002</v>
+        <v>26.126698000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -10859,10 +10439,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>31.097985999999999</v>
+        <v>36.860461999999998</v>
       </c>
       <c r="C11">
-        <v>30.99127</v>
+        <v>33.968029000000001</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -10870,10 +10450,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>31.399291999999999</v>
+        <v>37.069180000000003</v>
       </c>
       <c r="C12">
-        <v>32.092789000000003</v>
+        <v>35.946967999999998</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -10881,10 +10461,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>31.589500000000001</v>
+        <v>37.168762000000001</v>
       </c>
       <c r="C13">
-        <v>32.687973</v>
+        <v>36.622391</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -10892,10 +10472,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>31.729956000000001</v>
+        <v>37.284050000000001</v>
       </c>
       <c r="C14">
-        <v>33.095160999999997</v>
+        <v>36.980365999999997</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -10903,10 +10483,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>31.826536000000001</v>
+        <v>37.350613000000003</v>
       </c>
       <c r="C15">
-        <v>33.323334000000003</v>
+        <v>37.190429999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -10914,10 +10494,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>28.317527999999999</v>
+        <v>34.898707999999999</v>
       </c>
       <c r="C16">
-        <v>22.738938999999998</v>
+        <v>20.711213999999998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -10925,10 +10505,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>29.531122</v>
+        <v>35.442383</v>
       </c>
       <c r="C17">
-        <v>27.305260000000001</v>
+        <v>25.701533999999999</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -10936,10 +10516,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>29.914370999999999</v>
+        <v>35.476542999999999</v>
       </c>
       <c r="C18">
-        <v>28.801749999999998</v>
+        <v>32.268374999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -10947,10 +10527,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>30.1511</v>
+        <v>35.541428000000003</v>
       </c>
       <c r="C19">
-        <v>29.536162999999998</v>
+        <v>32.853240999999997</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -10958,10 +10538,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>30.318769</v>
+        <v>35.565033</v>
       </c>
       <c r="C20">
-        <v>30.126584999999999</v>
+        <v>33.024704</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -10969,10 +10549,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>30.407647999999998</v>
+        <v>35.543807999999999</v>
       </c>
       <c r="C21">
-        <v>30.388870000000001</v>
+        <v>33.015647999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -10980,10 +10560,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>30.475828</v>
+        <v>35.510756999999998</v>
       </c>
       <c r="C22">
-        <v>30.692335</v>
+        <v>32.982219999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>